<commit_message>
Change to Inner Compass Add Visual Corner
</commit_message>
<xml_diff>
--- a/assets/xls/2020-08-23-unicorns-race.xlsx
+++ b/assets/xls/2020-08-23-unicorns-race.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Siddharth\minima\assets\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8182D85A-1FBF-4798-8AAD-55CE021A65A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0E30F6-79F7-4AD1-AC55-72E5C844582A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A8DF3A75-44EE-44E8-8510-0F1633397F31}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{A8DF3A75-44EE-44E8-8510-0F1633397F31}"/>
   </bookViews>
   <sheets>
     <sheet name="Unicorns" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
-    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="2" r:id="rId6"/>
+    <pivotCache cacheId="3" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -8462,7 +8462,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -8495,7 +8494,6 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -8752,6 +8750,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-A448-4322-87DE-D5EF23B795B5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -8767,6 +8770,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-A448-4322-87DE-D5EF23B795B5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -8782,6 +8790,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-A448-4322-87DE-D5EF23B795B5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -8797,6 +8810,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-A448-4322-87DE-D5EF23B795B5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -8812,6 +8830,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-A448-4322-87DE-D5EF23B795B5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -8827,6 +8850,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-A448-4322-87DE-D5EF23B795B5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -8844,6 +8872,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-A448-4322-87DE-D5EF23B795B5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -8861,6 +8894,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-A448-4322-87DE-D5EF23B795B5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -8878,6 +8916,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-A448-4322-87DE-D5EF23B795B5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -8895,6 +8938,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000029-A448-4322-87DE-D5EF23B795B5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -8912,6 +8960,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002B-A448-4322-87DE-D5EF23B795B5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -20725,7 +20778,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4772FD7-BF22-411C-B225-1950229563E1}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4772FD7-BF22-411C-B225-1950229563E1}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField dataField="1" showAll="0"/>
@@ -20868,7 +20921,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0FF2B968-BCA1-48AF-B72E-013BF52B3D91}" name="PivotTable7" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0FF2B968-BCA1-48AF-B72E-013BF52B3D91}" name="PivotTable7" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B466" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -23508,8 +23561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B550BC-4EE3-4824-8C99-5CF84606C67F}">
   <dimension ref="B3:AK104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AA35" sqref="AA35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -26982,7 +27035,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="28.5">
+    <row r="104" spans="1:9">
       <c r="A104" s="7" t="s">
         <v>259</v>
       </c>
@@ -28616,7 +28669,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="28.5">
+    <row r="168" spans="1:8">
       <c r="A168" s="7" t="s">
         <v>378</v>
       </c>
@@ -30791,7 +30844,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="255" spans="1:9" ht="28.5">
+    <row r="255" spans="1:9">
       <c r="A255" s="7" t="s">
         <v>532</v>
       </c>
@@ -31616,7 +31669,7 @@
         <v>1438</v>
       </c>
     </row>
-    <row r="288" spans="1:9" ht="19.149999999999999">
+    <row r="288" spans="1:9">
       <c r="A288" s="7" t="s">
         <v>591</v>
       </c>
@@ -32591,7 +32644,7 @@
         <v>1491</v>
       </c>
     </row>
-    <row r="327" spans="1:9" ht="42.75">
+    <row r="327" spans="1:9" ht="28.5">
       <c r="A327" s="7" t="s">
         <v>658</v>
       </c>
@@ -33024,7 +33077,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="344" spans="1:8" ht="57">
+    <row r="344" spans="1:8" ht="42.75">
       <c r="A344" s="7" t="s">
         <v>689</v>
       </c>
@@ -33607,7 +33660,7 @@
         <v>1540</v>
       </c>
     </row>
-    <row r="367" spans="1:9" ht="28.5">
+    <row r="367" spans="1:9">
       <c r="A367" s="7" t="s">
         <v>727</v>
       </c>
@@ -33844,7 +33897,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="376" spans="1:8" ht="28.5">
+    <row r="376" spans="1:8">
       <c r="A376" s="7" t="s">
         <v>741</v>
       </c>
@@ -35363,7 +35416,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="435" spans="1:8" ht="28.5">
+    <row r="435" spans="1:8">
       <c r="A435" s="7" t="s">
         <v>846</v>
       </c>
@@ -36436,7 +36489,7 @@
         <v>1691</v>
       </c>
     </row>
-    <row r="478" spans="1:9" ht="28.5">
+    <row r="478" spans="1:9">
       <c r="A478" s="7" t="s">
         <v>920</v>
       </c>

</xml_diff>